<commit_message>
changed merging for some params
Изменил логику объединения и хранения значений для некоторых полей у задач. Теперь они принадлежат задаче, а не группе.

При заполнении объединяем только последовательно идущие строки с одинаковыми значениями.
</commit_message>
<xml_diff>
--- a/welding-report/Resources/Templates/SuprReportTemplate.xlsx
+++ b/welding-report/Resources/Templates/SuprReportTemplate.xlsx
@@ -65,11 +65,11 @@
     <t>Приоритет (потребность в изготовлении в 2024 г)</t>
   </si>
   <si>
-    <t>Заявка на локализацию оборудования и ЗИП № 41 от __.__ 20__г</t>
-  </si>
-  <si>
     <t>Деталь/
 сборочная единица</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Заявка на локализацию оборудования и ЗИП № </t>
   </si>
 </sst>
 </file>
@@ -234,6 +234,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -241,15 +250,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -543,7 +543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,83 +563,83 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="21" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="H5" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="I7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
@@ -651,10 +651,10 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="11"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>

</xml_diff>